<commit_message>
combining lab spikes and instrument check tables for all qc checks and update parameter file
</commit_message>
<xml_diff>
--- a/inst/extdata/ParameterMapping.xlsx
+++ b/inst/extdata/ParameterMapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Example input files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92B094D-7D92-4A93-8E7C-9DCA19D097DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E7FEED-52A8-42E9-9946-91C05C3BE52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
   </bookViews>
@@ -54,12 +54,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{9382D8ED-DD9E-41EA-8F4F-8DC06952F881}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>s.u. not valid for WQX</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{6A4C2D86-C342-4684-AE41-617AA2995846}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ppt not valid for WQX</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="93">
   <si>
     <t>Water Temp</t>
   </si>
@@ -250,9 +278,6 @@
     <t>uS/cm, mS/cm, S/m</t>
   </si>
   <si>
-    <t>ppth, PSU, PSS, g/kg</t>
-  </si>
-  <si>
     <t>Chl a</t>
   </si>
   <si>
@@ -277,15 +302,6 @@
     <t>Chlorophyll a (probe)</t>
   </si>
   <si>
-    <t>blank</t>
-  </si>
-  <si>
-    <t>If s.u. is used, switch it to blank for WQX.</t>
-  </si>
-  <si>
-    <t>If ppt is used, switch it to ppth for WQX.</t>
-  </si>
-  <si>
     <t>Microcystins</t>
   </si>
   <si>
@@ -307,13 +323,49 @@
     <t>PON</t>
   </si>
   <si>
-    <t>Method</t>
-  </si>
-  <si>
-    <t>Lab</t>
-  </si>
-  <si>
-    <t>InSitu</t>
+    <t>blank, s.u.</t>
+  </si>
+  <si>
+    <t>ppth, PSU, PSS, g/kg, ppt</t>
+  </si>
+  <si>
+    <t>Method Speciation</t>
+  </si>
+  <si>
+    <t>as P</t>
+  </si>
+  <si>
+    <t>as N</t>
+  </si>
+  <si>
+    <t>as S</t>
+  </si>
+  <si>
+    <t>as Si</t>
+  </si>
+  <si>
+    <t>as Cl</t>
+  </si>
+  <si>
+    <t>Result Sample Fraction</t>
+  </si>
+  <si>
+    <t>Unfiltered</t>
+  </si>
+  <si>
+    <t>Filtered, lab</t>
+  </si>
+  <si>
+    <t>Carbon</t>
+  </si>
+  <si>
+    <t>POC</t>
+  </si>
+  <si>
+    <t>Particulate organic carbon</t>
+  </si>
+  <si>
+    <t>as C</t>
   </si>
 </sst>
 </file>
@@ -706,13 +758,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84032A94-31D2-4739-AFB0-3D4EF11D54E8}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,8 +772,9 @@
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="58.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="59.28515625" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -734,11 +787,14 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -751,10 +807,7 @@
       <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -768,15 +821,10 @@
       <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="D3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -788,10 +836,7 @@
       <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -805,10 +850,7 @@
       <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -822,10 +864,7 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -839,10 +878,7 @@
       <c r="C7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -856,15 +892,10 @@
       <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>74</v>
-      </c>
+      <c r="D8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -876,11 +907,14 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>68</v>
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -893,11 +927,14 @@
       <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>68</v>
+      <c r="D10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -910,11 +947,14 @@
       <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>68</v>
+      <c r="D11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -922,16 +962,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>68</v>
+      <c r="D12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -944,11 +987,14 @@
       <c r="C13" t="s">
         <v>32</v>
       </c>
-      <c r="D13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>68</v>
+      <c r="D13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -961,11 +1007,14 @@
       <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="D14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>68</v>
+      <c r="D14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -978,11 +1027,14 @@
       <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>68</v>
+      <c r="D15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -995,14 +1047,17 @@
       <c r="C16" t="s">
         <v>41</v>
       </c>
-      <c r="D16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1012,31 +1067,37 @@
       <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="D17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1046,14 +1107,17 @@
       <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="D19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1063,350 +1127,355 @@
       <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>40</v>
       </c>
-      <c r="D25" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>43</v>
       </c>
-      <c r="D27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>53</v>
       </c>
-      <c r="D30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>17</v>
       </c>
-      <c r="D33" t="s">
-        <v>83</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>65</v>
+        <v>72</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>75</v>
+      <c r="B37" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>23</v>
       </c>
-      <c r="D39" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>47</v>
       </c>
-      <c r="D40" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
template updates and path changes on resources markdown file
</commit_message>
<xml_diff>
--- a/inst/extdata/ParameterMapping.xlsx
+++ b/inst/extdata/ParameterMapping.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E7FEED-52A8-42E9-9946-91C05C3BE52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B737CF-3D0D-4139-AF43-5BAD6B2C9F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Parameters" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +50,35 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Lighter shade represents less common parameters.  Might not need to include in analysis graphs.</t>
+          <t>Lighter shade represents less common parameters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{DC7BBA68-A3BF-42F0-B447-89A856725E74}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>For reference/default only.  Defined in WQX Meta file.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{FCC65F38-24FB-45EC-BAE0-229E25DA31B6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>For reference/default only.  Defined in WQX Meta file.</t>
         </r>
       </text>
     </comment>
@@ -64,7 +92,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>s.u. not valid for WQX</t>
+          <t>s.u. not valid for WQX.  Replace with blank.</t>
         </r>
       </text>
     </comment>
@@ -78,7 +106,49 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>ppt not valid for WQX</t>
+          <t>ppt not valid for WQX.  Replace with ppth.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{854A6E9E-DEF9-47F7-8425-35341E679C5A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If WQX parameter "Total Phosphorus, mixed forms" is supplied, then assume it is TP, not TDP.  User must supply TDP for this parameter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{A9C16E11-4BFE-423F-9D10-72D13758A7EF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If WQX parameter Total Nitrogen, mixed forms in supplied, then assume it is TN, not PON.  User must supply PON for this parameter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{8758E420-D1A5-4E25-B71C-B7DA476BB408}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If WQX parameter Total Nitrogen, mixed forms in supplied, then assume it is TN, not TDN.  User must supply TDN for this parameter.</t>
         </r>
       </text>
     </comment>
@@ -87,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="90">
   <si>
     <t>Water Temp</t>
   </si>
@@ -236,12 +306,6 @@
     <t>Specific conductance</t>
   </si>
   <si>
-    <t>Phosphate-phosphorus</t>
-  </si>
-  <si>
-    <t>Phosphate</t>
-  </si>
-  <si>
     <t>Phosphorus, Particulate Organic</t>
   </si>
   <si>
@@ -317,9 +381,6 @@
     <t>Silicate</t>
   </si>
   <si>
-    <t>Total Particulate Organic Nitrogen</t>
-  </si>
-  <si>
     <t>PON</t>
   </si>
   <si>
@@ -338,15 +399,6 @@
     <t>as N</t>
   </si>
   <si>
-    <t>as S</t>
-  </si>
-  <si>
-    <t>as Si</t>
-  </si>
-  <si>
-    <t>as Cl</t>
-  </si>
-  <si>
     <t>Result Sample Fraction</t>
   </si>
   <si>
@@ -365,24 +417,26 @@
     <t>Particulate organic carbon</t>
   </si>
   <si>
-    <t>as C</t>
+    <t>Suspended</t>
+  </si>
+  <si>
+    <t>TDN</t>
+  </si>
+  <si>
+    <t>TDP</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -394,8 +448,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,6 +487,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -433,12 +506,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,13 +832,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84032A94-31D2-4739-AFB0-3D4EF11D54E8}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,8 +847,8 @@
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="58.28515625" customWidth="1"/>
     <col min="4" max="4" width="59.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -788,13 +862,13 @@
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
         <v>80</v>
-      </c>
-      <c r="F1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -808,7 +882,13 @@
         <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -822,9 +902,14 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -837,7 +922,13 @@
         <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -851,7 +942,13 @@
         <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -865,7 +962,13 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -879,7 +982,13 @@
         <v>48</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -893,9 +1002,14 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -908,13 +1022,13 @@
         <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
         <v>81</v>
-      </c>
-      <c r="F9" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -922,59 +1036,59 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
         <v>81</v>
-      </c>
-      <c r="F10" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>50</v>
+      <c r="B11" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="C11" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
+      <c r="B12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -988,33 +1102,33 @@
         <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1028,13 +1142,13 @@
         <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1048,13 +1162,13 @@
         <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1068,53 +1182,53 @@
         <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>76</v>
+      <c r="B18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" t="s">
         <v>82</v>
-      </c>
-      <c r="F19" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1122,116 +1236,119 @@
         <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>90</v>
+        <v>31</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="F21" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>75</v>
+        <v>83</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>6</v>
+        <v>73</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F23" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>74</v>
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F24" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>4</v>
+        <v>72</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="E25" t="s">
+        <v>89</v>
       </c>
       <c r="F25" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1239,61 +1356,79 @@
         <v>46</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
       </c>
       <c r="F26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>19</v>
+      <c r="B28" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="E28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>18</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
+      </c>
+      <c r="E29" t="s">
+        <v>89</v>
       </c>
       <c r="F29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1301,47 +1436,59 @@
         <v>12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="E30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>54</v>
+      <c r="B31" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="E31" t="s">
+        <v>89</v>
       </c>
       <c r="F31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>89</v>
       </c>
       <c r="F32" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1349,61 +1496,79 @@
         <v>21</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="E33" t="s">
+        <v>89</v>
       </c>
       <c r="F33" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>17</v>
+      <c r="B34" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="E34" t="s">
+        <v>89</v>
       </c>
       <c r="F34" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>72</v>
+        <v>21</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="E35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="E36" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1411,72 +1576,119 @@
         <v>20</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="E37" t="s">
+        <v>89</v>
       </c>
       <c r="F37" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>71</v>
+      <c r="B38" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>73</v>
+        <v>20</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="E39" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>23</v>
+        <v>71</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="E40" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" t="s">
+        <v>89</v>
+      </c>
+      <c r="F41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>59</v>
+      <c r="D42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update parameter mapping with ph units
</commit_message>
<xml_diff>
--- a/inst/extdata/ParameterMapping.xlsx
+++ b/inst/extdata/ParameterMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A376F8CF-0003-4568-BED8-23DC47F77A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E9221A-2E94-4B84-B205-247B9CC799B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>s.u. not valid for WQX.  Replace with blank.</t>
+          <t>blank and s.u. not valid for WQX.  Replace with "None".</t>
         </r>
       </text>
     </comment>
@@ -356,9 +356,6 @@
     <t>PON</t>
   </si>
   <si>
-    <t>blank, s.u.</t>
-  </si>
-  <si>
     <t>ppth, PSU, PSS, g/kg, ppt</t>
   </si>
   <si>
@@ -390,13 +387,36 @@
   </si>
   <si>
     <t>Temperature, air</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>blank</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, s.u., None</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,6 +437,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -791,21 +819,21 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="58.28515625" customWidth="1"/>
-    <col min="4" max="4" width="59.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" customWidth="1"/>
+    <col min="3" max="3" width="58.26953125" customWidth="1"/>
+    <col min="4" max="4" width="59.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -819,7 +847,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -833,7 +861,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -844,10 +872,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -861,7 +889,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -875,7 +903,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -889,7 +917,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -903,7 +931,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -914,10 +942,10 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -931,7 +959,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -945,7 +973,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -959,12 +987,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>35</v>
@@ -973,7 +1001,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -987,7 +1015,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1001,7 +1029,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1015,7 +1043,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1029,7 +1057,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1043,7 +1071,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1057,12 +1085,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>41</v>
@@ -1071,7 +1099,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1085,7 +1113,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1099,21 +1127,21 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" t="s">
         <v>78</v>
       </c>
-      <c r="C22" t="s">
-        <v>79</v>
-      </c>
       <c r="D22" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1127,7 +1155,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1141,7 +1169,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1155,7 +1183,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1169,7 +1197,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -1183,7 +1211,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1197,7 +1225,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1211,7 +1239,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1225,7 +1253,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1239,7 +1267,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1253,7 +1281,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1267,7 +1295,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -1281,7 +1309,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1295,7 +1323,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1309,7 +1337,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -1323,7 +1351,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -1337,7 +1365,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -1351,7 +1379,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -1365,7 +1393,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -1379,9 +1407,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>47</v>
@@ -1393,29 +1421,29 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" t="s">
         <v>82</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" t="s">
-        <v>83</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
         <v>85</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" t="s">
-        <v>86</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
update parameter list with chl probe, phycocyanin, and phycoerythrin #67
</commit_message>
<xml_diff>
--- a/inst/extdata/ParameterMapping.xlsx
+++ b/inst/extdata/ParameterMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E9221A-2E94-4B84-B205-247B9CC799B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EDA553-5819-40F5-A5AC-3AD1AAD9AAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="92">
   <si>
     <t>Water Temp</t>
   </si>
@@ -410,6 +410,21 @@
       </rPr>
       <t>, s.u., None</t>
     </r>
+  </si>
+  <si>
+    <t>mg/l, ug/l, umol/l, ppm, RFU</t>
+  </si>
+  <si>
+    <t>Phycocyanin</t>
+  </si>
+  <si>
+    <t>Phycocyanin (probe)</t>
+  </si>
+  <si>
+    <t>Phycoerythrin</t>
+  </si>
+  <si>
+    <t>Phcyocyanin (probe)</t>
   </si>
 </sst>
 </file>
@@ -520,9 +535,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -560,7 +575,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -666,7 +681,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -808,7 +823,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -816,24 +831,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84032A94-31D2-4739-AFB0-3D4EF11D54E8}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" customWidth="1"/>
-    <col min="3" max="3" width="58.26953125" customWidth="1"/>
-    <col min="4" max="4" width="59.26953125" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" customWidth="1"/>
+    <col min="3" max="3" width="58.21875" customWidth="1"/>
+    <col min="4" max="4" width="59.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -847,7 +862,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -861,7 +876,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -875,7 +890,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -889,7 +904,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -903,7 +918,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -917,7 +932,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -931,7 +946,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -945,7 +960,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -959,7 +974,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -973,7 +988,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -987,7 +1002,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1001,7 +1016,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1015,7 +1030,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1029,7 +1044,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1043,7 +1058,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1057,7 +1072,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1071,7 +1086,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1085,7 +1100,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1099,7 +1114,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1113,7 +1128,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1127,7 +1142,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -1141,7 +1156,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1155,7 +1170,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1169,7 +1184,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1183,7 +1198,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1197,7 +1212,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -1211,7 +1226,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1225,7 +1240,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1239,7 +1254,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1253,7 +1268,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1264,10 +1279,10 @@
         <v>68</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1281,7 +1296,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1295,7 +1310,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -1309,7 +1324,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1323,7 +1338,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1337,7 +1352,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -1348,10 +1363,10 @@
         <v>44</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -1365,87 +1380,129 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C42" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="D42" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C43" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="D43" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C44" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C45" t="s">
         <v>47</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C46" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C47" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>